<commit_message>
Cleaned Data. Need to make plots
</commit_message>
<xml_diff>
--- a/cleaned_data/aggregated_data.xlsx
+++ b/cleaned_data/aggregated_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="189" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="189" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TTC per Pilot" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,6 @@
     <sheet name="Success Rate" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Incomplete Units" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Unexecuted Units" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Location" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -93,6 +92,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1305,7 +1305,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1695,7 +1695,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2985,7 +2985,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3000,7 +3000,7 @@
   </sheetPr>
   <dimension ref="A1:AI5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3344,7 +3344,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3357,10 +3357,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P18" activeCellId="0" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3421,10 +3421,374 @@
         <v>16</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>1028</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>263</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3437,10 +3801,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3501,36 +3865,374 @@
         <v>16</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>1022</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>263</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>